<commit_message>
Cambios en lab_mass y cambio en la columna delivery_date de masa_25.xlsx
</commit_message>
<xml_diff>
--- a/data/raw/masa_25.xlsx
+++ b/data/raw/masa_25.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Miguel Oscar\Projects\data-INSCO-hub\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C22B4C42-64AA-4A09-9905-A69DC40C7D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7EC7BB-7401-43EC-998D-87D0620634A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1843,9 +1843,6 @@
     <t>calibration_date</t>
   </si>
   <si>
-    <t xml:space="preserve">delivery_date </t>
-  </si>
-  <si>
     <t>delivery_time</t>
   </si>
   <si>
@@ -1907,6 +1904,9 @@
   </si>
   <si>
     <t>assignee</t>
+  </si>
+  <si>
+    <t>delivery_date</t>
   </si>
 </sst>
 </file>
@@ -2268,11 +2268,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:T586"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A520" workbookViewId="0">
-      <selection activeCell="C547" sqref="C547:D547"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2302,7 +2301,7 @@
         <v>596</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>597</v>
@@ -2329,34 +2328,34 @@
         <v>604</v>
       </c>
       <c r="L1" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>605</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>610</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>611</v>
       </c>
-      <c r="T1" s="1" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -2416,7 +2415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -2476,7 +2475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -2536,7 +2535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -2596,9 +2595,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:20" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>12</v>
@@ -2658,9 +2657,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:20" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>1</v>
@@ -2720,7 +2719,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -2780,7 +2779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -2840,7 +2839,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>19</v>
       </c>
@@ -2900,7 +2899,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -2960,7 +2959,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -3020,7 +3019,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>28</v>
       </c>
@@ -3080,7 +3079,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>30</v>
       </c>
@@ -3140,7 +3139,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>32</v>
       </c>
@@ -3200,7 +3199,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>35</v>
       </c>
@@ -3260,7 +3259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>35</v>
       </c>
@@ -3322,7 +3321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>39</v>
       </c>
@@ -3384,7 +3383,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>39</v>
       </c>
@@ -3444,7 +3443,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>40</v>
       </c>
@@ -3506,7 +3505,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
@@ -3566,7 +3565,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>41</v>
       </c>
@@ -3626,7 +3625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>43</v>
       </c>
@@ -3686,7 +3685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>44</v>
       </c>
@@ -3746,7 +3745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>46</v>
       </c>
@@ -3806,7 +3805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>47</v>
       </c>
@@ -3866,7 +3865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>48</v>
       </c>
@@ -3926,7 +3925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>49</v>
       </c>
@@ -3986,7 +3985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>50</v>
       </c>
@@ -4046,7 +4045,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>51</v>
       </c>
@@ -4106,9 +4105,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>53</v>
@@ -4168,9 +4167,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>55</v>
@@ -4230,7 +4229,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>57</v>
       </c>
@@ -4290,7 +4289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>60</v>
       </c>
@@ -4350,7 +4349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>62</v>
       </c>
@@ -4410,7 +4409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>63</v>
       </c>
@@ -4470,7 +4469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>64</v>
       </c>
@@ -4530,7 +4529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>65</v>
       </c>
@@ -4590,7 +4589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>66</v>
       </c>
@@ -4650,7 +4649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>67</v>
       </c>
@@ -4710,7 +4709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>68</v>
       </c>
@@ -4770,7 +4769,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>69</v>
       </c>
@@ -4830,7 +4829,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>71</v>
       </c>
@@ -4890,7 +4889,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>72</v>
       </c>
@@ -4950,7 +4949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>74</v>
       </c>
@@ -5010,7 +5009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>75</v>
       </c>
@@ -5072,7 +5071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>80</v>
       </c>
@@ -5132,7 +5131,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>82</v>
       </c>
@@ -5194,7 +5193,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>82</v>
       </c>
@@ -5254,7 +5253,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="50" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>85</v>
       </c>
@@ -5314,7 +5313,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>86</v>
       </c>
@@ -5374,7 +5373,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>88</v>
       </c>
@@ -5436,7 +5435,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>88</v>
       </c>
@@ -5496,7 +5495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>88</v>
       </c>
@@ -5558,7 +5557,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>91</v>
       </c>
@@ -5618,7 +5617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>93</v>
       </c>
@@ -5678,7 +5677,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>94</v>
       </c>
@@ -5738,7 +5737,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>95</v>
       </c>
@@ -5798,7 +5797,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>97</v>
       </c>
@@ -5858,7 +5857,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>98</v>
       </c>
@@ -5918,7 +5917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>101</v>
       </c>
@@ -5978,7 +5977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>102</v>
       </c>
@@ -6038,7 +6037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>104</v>
       </c>
@@ -6098,7 +6097,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>105</v>
       </c>
@@ -6158,7 +6157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>106</v>
       </c>
@@ -6218,7 +6217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>107</v>
       </c>
@@ -6278,7 +6277,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>109</v>
       </c>
@@ -6338,7 +6337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>110</v>
       </c>
@@ -6398,7 +6397,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>112</v>
       </c>
@@ -6458,7 +6457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>112</v>
       </c>
@@ -6520,7 +6519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>112</v>
       </c>
@@ -6582,7 +6581,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>112</v>
       </c>
@@ -6632,7 +6631,7 @@
         <v>6</v>
       </c>
       <c r="Q72" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="R72" s="2" t="s">
         <v>116</v>
@@ -6644,7 +6643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>112</v>
       </c>
@@ -6706,7 +6705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>117</v>
       </c>
@@ -6768,7 +6767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>120</v>
       </c>
@@ -6830,7 +6829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" s="2" t="s">
         <v>122</v>
       </c>
@@ -6890,7 +6889,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>124</v>
       </c>
@@ -6950,7 +6949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>125</v>
       </c>
@@ -7010,7 +7009,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>126</v>
       </c>
@@ -7070,7 +7069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>127</v>
       </c>
@@ -7130,7 +7129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>128</v>
       </c>
@@ -7190,7 +7189,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>129</v>
       </c>
@@ -7250,7 +7249,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="83" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>131</v>
       </c>
@@ -7310,7 +7309,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>133</v>
       </c>
@@ -7370,7 +7369,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>135</v>
       </c>
@@ -7430,7 +7429,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>137</v>
       </c>
@@ -7490,7 +7489,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>139</v>
       </c>
@@ -7550,7 +7549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>141</v>
       </c>
@@ -7610,7 +7609,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>142</v>
       </c>
@@ -7670,7 +7669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="2" t="s">
         <v>144</v>
       </c>
@@ -7730,7 +7729,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A91" s="2" t="s">
         <v>145</v>
       </c>
@@ -7790,7 +7789,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="92" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A92" s="2" t="s">
         <v>146</v>
       </c>
@@ -7850,7 +7849,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="93" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="2" t="s">
         <v>147</v>
       </c>
@@ -7910,7 +7909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" s="2" t="s">
         <v>148</v>
       </c>
@@ -7970,7 +7969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A95" s="2" t="s">
         <v>150</v>
       </c>
@@ -8030,7 +8029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="2" t="s">
         <v>151</v>
       </c>
@@ -8090,7 +8089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" s="2" t="s">
         <v>152</v>
       </c>
@@ -8150,7 +8149,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
         <v>153</v>
       </c>
@@ -8210,7 +8209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
         <v>154</v>
       </c>
@@ -8270,7 +8269,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
         <v>155</v>
       </c>
@@ -8330,7 +8329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A101" s="2" t="s">
         <v>156</v>
       </c>
@@ -8392,7 +8391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A102" s="2" t="s">
         <v>156</v>
       </c>
@@ -8452,7 +8451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A103" s="2" t="s">
         <v>157</v>
       </c>
@@ -8514,7 +8513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A104" s="2" t="s">
         <v>157</v>
       </c>
@@ -8574,7 +8573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A105" s="2" t="s">
         <v>158</v>
       </c>
@@ -8634,7 +8633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="2" t="s">
         <v>161</v>
       </c>
@@ -8694,7 +8693,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A107" s="2" t="s">
         <v>163</v>
       </c>
@@ -8754,7 +8753,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" s="2" t="s">
         <v>164</v>
       </c>
@@ -8814,7 +8813,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A109" s="2" t="s">
         <v>165</v>
       </c>
@@ -8822,7 +8821,7 @@
         <v>166</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>59</v>
@@ -8874,7 +8873,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="110" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A110" s="2" t="s">
         <v>167</v>
       </c>
@@ -8934,7 +8933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="2" t="s">
         <v>169</v>
       </c>
@@ -8994,7 +8993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="2" t="s">
         <v>170</v>
       </c>
@@ -9054,7 +9053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" s="2" t="s">
         <v>172</v>
       </c>
@@ -9114,7 +9113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" s="2" t="s">
         <v>173</v>
       </c>
@@ -9174,7 +9173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" s="2" t="s">
         <v>174</v>
       </c>
@@ -9234,7 +9233,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="116" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A116" s="2" t="s">
         <v>176</v>
       </c>
@@ -9294,7 +9293,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" s="2" t="s">
         <v>178</v>
       </c>
@@ -9354,7 +9353,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="118" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A118" s="2" t="s">
         <v>180</v>
       </c>
@@ -9414,7 +9413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
         <v>183</v>
       </c>
@@ -9474,7 +9473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
         <v>184</v>
       </c>
@@ -9534,7 +9533,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="121" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A121" s="2" t="s">
         <v>186</v>
       </c>
@@ -9592,7 +9591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>188</v>
       </c>
@@ -9652,7 +9651,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="123" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="2" t="s">
         <v>190</v>
       </c>
@@ -9712,7 +9711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A124" s="2" t="s">
         <v>192</v>
       </c>
@@ -9772,7 +9771,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="125" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" s="2" t="s">
         <v>194</v>
       </c>
@@ -9832,7 +9831,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="126" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A126" s="2" t="s">
         <v>196</v>
       </c>
@@ -9892,7 +9891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" s="2" t="s">
         <v>197</v>
       </c>
@@ -9952,7 +9951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
         <v>199</v>
       </c>
@@ -10012,7 +10011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>200</v>
       </c>
@@ -10072,7 +10071,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="130" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>201</v>
       </c>
@@ -10132,7 +10131,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="131" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>203</v>
       </c>
@@ -10192,7 +10191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>205</v>
       </c>
@@ -10252,7 +10251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>206</v>
       </c>
@@ -10312,7 +10311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>207</v>
       </c>
@@ -10372,7 +10371,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>208</v>
       </c>
@@ -10432,9 +10431,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B136" s="2" t="s">
         <v>210</v>
@@ -10492,9 +10491,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B137" s="2" t="s">
         <v>210</v>
@@ -10552,7 +10551,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="138" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>211</v>
       </c>
@@ -10612,7 +10611,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>213</v>
       </c>
@@ -10672,7 +10671,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="140" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>215</v>
       </c>
@@ -10732,7 +10731,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="141" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>216</v>
       </c>
@@ -10792,7 +10791,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="142" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>217</v>
       </c>
@@ -10852,7 +10851,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="143" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>219</v>
       </c>
@@ -10912,7 +10911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>221</v>
       </c>
@@ -10972,7 +10971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A145" s="2" t="s">
         <v>222</v>
       </c>
@@ -11032,7 +11031,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
         <v>223</v>
       </c>
@@ -11092,7 +11091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
         <v>224</v>
       </c>
@@ -11152,7 +11151,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A148" s="2" t="s">
         <v>225</v>
       </c>
@@ -11212,9 +11211,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A149" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B149" s="2" t="s">
         <v>226</v>
@@ -11272,9 +11271,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="150" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A150" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="B150" s="2" t="s">
         <v>226</v>
@@ -11332,7 +11331,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="151" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A151" s="2" t="s">
         <v>227</v>
       </c>
@@ -11392,7 +11391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A152" s="2" t="s">
         <v>229</v>
       </c>
@@ -11452,7 +11451,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A153" s="2" t="s">
         <v>230</v>
       </c>
@@ -11512,7 +11511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A154" s="2" t="s">
         <v>230</v>
       </c>
@@ -11574,7 +11573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A155" s="2" t="s">
         <v>231</v>
       </c>
@@ -11634,7 +11633,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="156" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A156" s="2" t="s">
         <v>232</v>
       </c>
@@ -11694,7 +11693,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="157" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A157" s="2" t="s">
         <v>234</v>
       </c>
@@ -11754,7 +11753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A158" s="2" t="s">
         <v>236</v>
       </c>
@@ -11814,7 +11813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A159" s="2" t="s">
         <v>237</v>
       </c>
@@ -11874,7 +11873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
         <v>238</v>
       </c>
@@ -11934,7 +11933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A161" s="2" t="s">
         <v>240</v>
       </c>
@@ -11994,7 +11993,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A162" s="2" t="s">
         <v>241</v>
       </c>
@@ -12054,7 +12053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="163" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A163" s="2" t="s">
         <v>242</v>
       </c>
@@ -12114,7 +12113,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A164" s="2" t="s">
         <v>243</v>
       </c>
@@ -12174,7 +12173,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="165" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" s="2" t="s">
         <v>244</v>
       </c>
@@ -12234,7 +12233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="166" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A166" s="2" t="s">
         <v>246</v>
       </c>
@@ -12294,7 +12293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A167" s="2" t="s">
         <v>247</v>
       </c>
@@ -12354,7 +12353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="168" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
         <v>248</v>
       </c>
@@ -12414,7 +12413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A169" s="2" t="s">
         <v>250</v>
       </c>
@@ -12474,7 +12473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="170" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
         <v>251</v>
       </c>
@@ -12534,7 +12533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A171" s="2" t="s">
         <v>252</v>
       </c>
@@ -12594,7 +12593,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="172" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A172" s="2" t="s">
         <v>255</v>
       </c>
@@ -12654,7 +12653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="173" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A173" s="2" t="s">
         <v>258</v>
       </c>
@@ -12714,7 +12713,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="174" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A174" s="2" t="s">
         <v>259</v>
       </c>
@@ -12774,7 +12773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A175" s="2" t="s">
         <v>261</v>
       </c>
@@ -12834,7 +12833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A176" s="2" t="s">
         <v>262</v>
       </c>
@@ -12894,7 +12893,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="177" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A177" s="2" t="s">
         <v>264</v>
       </c>
@@ -12954,7 +12953,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="178" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A178" s="2" t="s">
         <v>266</v>
       </c>
@@ -13016,7 +13015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A179" s="2" t="s">
         <v>269</v>
       </c>
@@ -13078,7 +13077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A180" s="2" t="s">
         <v>270</v>
       </c>
@@ -13138,7 +13137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A181" s="2" t="s">
         <v>272</v>
       </c>
@@ -13198,7 +13197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A182" s="2" t="s">
         <v>273</v>
       </c>
@@ -13258,7 +13257,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="183" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A183" s="2" t="s">
         <v>274</v>
       </c>
@@ -13318,7 +13317,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="184" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A184" s="2" t="s">
         <v>274</v>
       </c>
@@ -13380,7 +13379,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="185" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A185" s="2" t="s">
         <v>276</v>
       </c>
@@ -13440,7 +13439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A186" s="2" t="s">
         <v>278</v>
       </c>
@@ -13500,7 +13499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
         <v>279</v>
       </c>
@@ -13560,7 +13559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A188" s="2" t="s">
         <v>280</v>
       </c>
@@ -13620,7 +13619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A189" s="2" t="s">
         <v>281</v>
       </c>
@@ -13680,7 +13679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="190" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A190" s="2" t="s">
         <v>283</v>
       </c>
@@ -13740,7 +13739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A191" s="2" t="s">
         <v>284</v>
       </c>
@@ -13800,7 +13799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="192" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A192" s="2" t="s">
         <v>285</v>
       </c>
@@ -13860,7 +13859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="193" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A193" s="2" t="s">
         <v>286</v>
       </c>
@@ -13920,7 +13919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="194" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A194" s="2" t="s">
         <v>287</v>
       </c>
@@ -13980,7 +13979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A195" s="2" t="s">
         <v>288</v>
       </c>
@@ -14040,7 +14039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="196" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A196" s="2" t="s">
         <v>289</v>
       </c>
@@ -14100,7 +14099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="197" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
         <v>291</v>
       </c>
@@ -14160,7 +14159,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="198" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A198" s="2" t="s">
         <v>293</v>
       </c>
@@ -14220,7 +14219,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="199" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
         <v>295</v>
       </c>
@@ -14280,7 +14279,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="200" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A200" s="2" t="s">
         <v>296</v>
       </c>
@@ -14340,7 +14339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A201" s="2" t="s">
         <v>298</v>
       </c>
@@ -14398,7 +14397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="202" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A202" s="2" t="s">
         <v>299</v>
       </c>
@@ -14458,7 +14457,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="203" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A203" s="2" t="s">
         <v>301</v>
       </c>
@@ -14518,7 +14517,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="204" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A204" s="2" t="s">
         <v>303</v>
       </c>
@@ -14578,7 +14577,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="205" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A205" s="2" t="s">
         <v>305</v>
       </c>
@@ -14638,7 +14637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="206" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
         <v>307</v>
       </c>
@@ -14698,7 +14697,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="207" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A207" s="2" t="s">
         <v>309</v>
       </c>
@@ -14760,7 +14759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
         <v>311</v>
       </c>
@@ -14820,7 +14819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="209" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>312</v>
       </c>
@@ -14880,7 +14879,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>314</v>
       </c>
@@ -14940,7 +14939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>315</v>
       </c>
@@ -15000,7 +14999,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="212" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>317</v>
       </c>
@@ -15062,7 +15061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>320</v>
       </c>
@@ -15122,7 +15121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="214" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>322</v>
       </c>
@@ -15182,7 +15181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>323</v>
       </c>
@@ -15244,7 +15243,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="216" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>323</v>
       </c>
@@ -15304,7 +15303,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="217" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>325</v>
       </c>
@@ -15366,7 +15365,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="218" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>325</v>
       </c>
@@ -15426,7 +15425,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="219" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>326</v>
       </c>
@@ -15486,7 +15485,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="220" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>328</v>
       </c>
@@ -15546,7 +15545,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="221" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
         <v>329</v>
       </c>
@@ -15606,7 +15605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="222" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>330</v>
       </c>
@@ -15666,7 +15665,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="223" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
         <v>332</v>
       </c>
@@ -15726,7 +15725,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="224" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
         <v>334</v>
       </c>
@@ -15786,7 +15785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="225" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
         <v>335</v>
       </c>
@@ -15846,7 +15845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>336</v>
       </c>
@@ -15906,7 +15905,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="227" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
         <v>337</v>
       </c>
@@ -15966,7 +15965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="228" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
         <v>338</v>
       </c>
@@ -16026,7 +16025,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
         <v>339</v>
       </c>
@@ -16086,7 +16085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="230" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
         <v>340</v>
       </c>
@@ -16146,7 +16145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="231" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A231" s="2" t="s">
         <v>341</v>
       </c>
@@ -16206,7 +16205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A232" s="2" t="s">
         <v>342</v>
       </c>
@@ -16266,7 +16265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A233" s="2" t="s">
         <v>343</v>
       </c>
@@ -16326,7 +16325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A234" s="2" t="s">
         <v>344</v>
       </c>
@@ -16386,7 +16385,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A235" s="2" t="s">
         <v>345</v>
       </c>
@@ -16446,7 +16445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A236" s="2" t="s">
         <v>347</v>
       </c>
@@ -16506,7 +16505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="237" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A237" s="2" t="s">
         <v>349</v>
       </c>
@@ -16566,7 +16565,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A238" s="2" t="s">
         <v>350</v>
       </c>
@@ -16626,7 +16625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A239" s="2" t="s">
         <v>352</v>
       </c>
@@ -16686,7 +16685,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A240" s="2" t="s">
         <v>353</v>
       </c>
@@ -16746,7 +16745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A241" s="2" t="s">
         <v>354</v>
       </c>
@@ -16806,7 +16805,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="242" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A242" s="2" t="s">
         <v>355</v>
       </c>
@@ -16866,7 +16865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A243" s="2" t="s">
         <v>357</v>
       </c>
@@ -16926,7 +16925,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="244" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A244" s="2" t="s">
         <v>359</v>
       </c>
@@ -16986,7 +16985,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="245" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A245" s="2" t="s">
         <v>360</v>
       </c>
@@ -17046,7 +17045,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="246" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A246" s="2" t="s">
         <v>362</v>
       </c>
@@ -17106,7 +17105,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A247" s="2" t="s">
         <v>364</v>
       </c>
@@ -17166,7 +17165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A248" s="2" t="s">
         <v>365</v>
       </c>
@@ -17228,7 +17227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="249" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
         <v>368</v>
       </c>
@@ -17290,7 +17289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="250" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
         <v>369</v>
       </c>
@@ -17352,7 +17351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A251" s="2" t="s">
         <v>370</v>
       </c>
@@ -17414,7 +17413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="252" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A252" s="2" t="s">
         <v>371</v>
       </c>
@@ -17476,7 +17475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="253" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A253" s="2" t="s">
         <v>372</v>
       </c>
@@ -17538,7 +17537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A254" s="2" t="s">
         <v>373</v>
       </c>
@@ -17598,7 +17597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="255" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
         <v>375</v>
       </c>
@@ -17658,7 +17657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="256" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A256" s="2" t="s">
         <v>376</v>
       </c>
@@ -17718,7 +17717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A257" s="2" t="s">
         <v>377</v>
       </c>
@@ -17778,7 +17777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="258" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A258" s="2" t="s">
         <v>378</v>
       </c>
@@ -17838,7 +17837,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="259" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A259" s="2" t="s">
         <v>380</v>
       </c>
@@ -17898,7 +17897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="260" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A260" s="2" t="s">
         <v>381</v>
       </c>
@@ -17958,7 +17957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="261" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A261" s="2" t="s">
         <v>382</v>
       </c>
@@ -18018,7 +18017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A262" s="2" t="s">
         <v>383</v>
       </c>
@@ -18078,7 +18077,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A263" s="2" t="s">
         <v>384</v>
       </c>
@@ -18138,7 +18137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="264" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A264" s="2" t="s">
         <v>386</v>
       </c>
@@ -18198,7 +18197,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="265" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A265" s="2" t="s">
         <v>387</v>
       </c>
@@ -18258,7 +18257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="266" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A266" s="2" t="s">
         <v>389</v>
       </c>
@@ -18318,7 +18317,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="267" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A267" s="2" t="s">
         <v>391</v>
       </c>
@@ -18380,7 +18379,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="268" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A268" s="2" t="s">
         <v>394</v>
       </c>
@@ -18440,7 +18439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="269" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A269" s="2" t="s">
         <v>395</v>
       </c>
@@ -18500,7 +18499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="270" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A270" s="2" t="s">
         <v>396</v>
       </c>
@@ -18560,7 +18559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A271" s="2" t="s">
         <v>398</v>
       </c>
@@ -18620,7 +18619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="272" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A272" s="2" t="s">
         <v>400</v>
       </c>
@@ -18680,7 +18679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A273" s="2" t="s">
         <v>401</v>
       </c>
@@ -18740,7 +18739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A274" s="2" t="s">
         <v>402</v>
       </c>
@@ -18800,7 +18799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="275" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A275" s="2" t="s">
         <v>403</v>
       </c>
@@ -18860,7 +18859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="276" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A276" s="2" t="s">
         <v>404</v>
       </c>
@@ -18918,7 +18917,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="277" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A277" s="2" t="s">
         <v>407</v>
       </c>
@@ -18978,7 +18977,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="278" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A278" s="2" t="s">
         <v>409</v>
       </c>
@@ -19038,7 +19037,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A279" s="2" t="s">
         <v>411</v>
       </c>
@@ -19098,7 +19097,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A280" s="2" t="s">
         <v>412</v>
       </c>
@@ -19158,7 +19157,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="281" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A281" s="2" t="s">
         <v>413</v>
       </c>
@@ -19218,7 +19217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="282" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A282" s="2" t="s">
         <v>415</v>
       </c>
@@ -19278,7 +19277,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="283" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A283" s="2" t="s">
         <v>416</v>
       </c>
@@ -19338,7 +19337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="284" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A284" s="2" t="s">
         <v>417</v>
       </c>
@@ -19398,7 +19397,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="285" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A285" s="2" t="s">
         <v>418</v>
       </c>
@@ -19458,7 +19457,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="286" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A286" s="2" t="s">
         <v>420</v>
       </c>
@@ -19518,7 +19517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="287" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A287" s="2" t="s">
         <v>421</v>
       </c>
@@ -19578,7 +19577,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="288" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A288" s="2" t="s">
         <v>424</v>
       </c>
@@ -19638,7 +19637,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="289" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A289" s="2" t="s">
         <v>425</v>
       </c>
@@ -19698,9 +19697,9 @@
         <v>29</v>
       </c>
     </row>
-    <row r="290" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A290" s="2" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B290" s="2" t="s">
         <v>427</v>
@@ -19758,9 +19757,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="291" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A291" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B291" s="2" t="s">
         <v>427</v>
@@ -19818,7 +19817,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="292" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A292" s="2" t="s">
         <v>428</v>
       </c>
@@ -19878,7 +19877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="293" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A293" s="2" t="s">
         <v>430</v>
       </c>
@@ -19938,7 +19937,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="294" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A294" s="2" t="s">
         <v>431</v>
       </c>
@@ -19998,7 +19997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="295" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A295" s="2" t="s">
         <v>432</v>
       </c>
@@ -20058,7 +20057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="296" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A296" s="2" t="s">
         <v>434</v>
       </c>
@@ -20118,7 +20117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="297" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A297" s="2" t="s">
         <v>435</v>
       </c>
@@ -20178,7 +20177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="298" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A298" s="2" t="s">
         <v>436</v>
       </c>
@@ -20238,7 +20237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="299" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A299" s="2" t="s">
         <v>437</v>
       </c>
@@ -20298,7 +20297,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="300" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A300" s="2" t="s">
         <v>439</v>
       </c>
@@ -20358,7 +20357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="301" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A301" s="2" t="s">
         <v>441</v>
       </c>
@@ -20418,7 +20417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A302" s="2" t="s">
         <v>442</v>
       </c>
@@ -20480,7 +20479,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="303" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A303" s="2" t="s">
         <v>442</v>
       </c>
@@ -20540,7 +20539,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="304" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A304" s="2" t="s">
         <v>445</v>
       </c>
@@ -20600,7 +20599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="305" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A305" s="2" t="s">
         <v>447</v>
       </c>
@@ -20660,7 +20659,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="306" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A306" s="2" t="s">
         <v>449</v>
       </c>
@@ -20720,7 +20719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="307" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A307" s="2" t="s">
         <v>450</v>
       </c>
@@ -20780,7 +20779,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="308" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A308" s="2" t="s">
         <v>451</v>
       </c>
@@ -20840,7 +20839,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="309" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A309" s="2" t="s">
         <v>452</v>
       </c>
@@ -20900,7 +20899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="310" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A310" s="2" t="s">
         <v>454</v>
       </c>
@@ -20960,7 +20959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="311" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A311" s="2" t="s">
         <v>456</v>
       </c>
@@ -21020,7 +21019,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="312" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A312" s="2" t="s">
         <v>458</v>
       </c>
@@ -21080,7 +21079,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="313" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A313" s="2" t="s">
         <v>459</v>
       </c>
@@ -21140,7 +21139,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="314" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A314" s="2" t="s">
         <v>461</v>
       </c>
@@ -21200,7 +21199,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="315" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A315" s="2" t="s">
         <v>463</v>
       </c>
@@ -21260,7 +21259,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="316" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A316" s="2" t="s">
         <v>464</v>
       </c>
@@ -21320,7 +21319,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="317" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A317" s="2" t="s">
         <v>465</v>
       </c>
@@ -21380,7 +21379,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="318" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A318" s="2" t="s">
         <v>467</v>
       </c>
@@ -21440,7 +21439,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="319" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A319" s="2" t="s">
         <v>468</v>
       </c>
@@ -21500,7 +21499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="320" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A320" s="2" t="s">
         <v>470</v>
       </c>
@@ -21560,7 +21559,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="321" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A321" s="2" t="s">
         <v>471</v>
       </c>
@@ -21620,7 +21619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="322" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A322" s="2" t="s">
         <v>473</v>
       </c>
@@ -21680,7 +21679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="323" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A323" s="2" t="s">
         <v>474</v>
       </c>
@@ -21740,7 +21739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="324" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A324" s="2" t="s">
         <v>476</v>
       </c>
@@ -21800,7 +21799,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="325" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A325" s="2" t="s">
         <v>477</v>
       </c>
@@ -21860,7 +21859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="326" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A326" s="2" t="s">
         <v>478</v>
       </c>
@@ -21920,7 +21919,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="327" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A327" s="2" t="s">
         <v>478</v>
       </c>
@@ -21982,7 +21981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="328" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A328" s="2" t="s">
         <v>479</v>
       </c>
@@ -22044,7 +22043,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="329" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A329" s="2" t="s">
         <v>482</v>
       </c>
@@ -22104,7 +22103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="330" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A330" s="2" t="s">
         <v>484</v>
       </c>
@@ -22164,7 +22163,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="331" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A331" s="2" t="s">
         <v>485</v>
       </c>
@@ -22224,7 +22223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="332" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A332" s="2" t="s">
         <v>486</v>
       </c>
@@ -22284,7 +22283,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A333" s="2" t="s">
         <v>487</v>
       </c>
@@ -22344,7 +22343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="334" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A334" s="2" t="s">
         <v>488</v>
       </c>
@@ -22404,7 +22403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="335" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A335" s="2" t="s">
         <v>489</v>
       </c>
@@ -22464,7 +22463,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="336" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A336" s="2" t="s">
         <v>490</v>
       </c>
@@ -22524,7 +22523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="337" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A337" s="2" t="s">
         <v>492</v>
       </c>
@@ -22584,7 +22583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="338" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A338" s="2" t="s">
         <v>493</v>
       </c>
@@ -22644,7 +22643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A339" s="2" t="s">
         <v>494</v>
       </c>
@@ -22704,7 +22703,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="340" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A340" s="2" t="s">
         <v>495</v>
       </c>
@@ -22764,7 +22763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="341" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A341" s="2" t="s">
         <v>497</v>
       </c>
@@ -22824,7 +22823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="342" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A342" s="2" t="s">
         <v>498</v>
       </c>
@@ -22884,7 +22883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="343" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A343" s="2" t="s">
         <v>499</v>
       </c>
@@ -22944,7 +22943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="344" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A344" s="2" t="s">
         <v>500</v>
       </c>
@@ -23004,7 +23003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="345" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A345" s="2" t="s">
         <v>501</v>
       </c>
@@ -23064,7 +23063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="346" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A346" s="2" t="s">
         <v>502</v>
       </c>
@@ -23124,7 +23123,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="347" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A347" s="2" t="s">
         <v>503</v>
       </c>
@@ -23184,7 +23183,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="348" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A348" s="2" t="s">
         <v>504</v>
       </c>
@@ -23244,7 +23243,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="349" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A349" s="2" t="s">
         <v>506</v>
       </c>
@@ -23304,7 +23303,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="350" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A350" s="2" t="s">
         <v>507</v>
       </c>
@@ -23364,7 +23363,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="351" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A351" s="2" t="s">
         <v>508</v>
       </c>
@@ -23424,7 +23423,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="352" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A352" s="2" t="s">
         <v>510</v>
       </c>
@@ -23484,7 +23483,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="353" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A353" s="2" t="s">
         <v>512</v>
       </c>
@@ -23544,7 +23543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="354" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A354" s="2" t="s">
         <v>513</v>
       </c>
@@ -23604,7 +23603,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="355" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A355" s="2" t="s">
         <v>514</v>
       </c>
@@ -23664,7 +23663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="356" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A356" s="2" t="s">
         <v>515</v>
       </c>
@@ -23724,7 +23723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="357" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A357" s="2" t="s">
         <v>517</v>
       </c>
@@ -23784,7 +23783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="358" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A358" s="2" t="s">
         <v>519</v>
       </c>
@@ -23844,7 +23843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="359" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A359" s="2" t="s">
         <v>520</v>
       </c>
@@ -23904,7 +23903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="360" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A360" s="2" t="s">
         <v>522</v>
       </c>
@@ -23964,7 +23963,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="361" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A361" s="2" t="s">
         <v>524</v>
       </c>
@@ -24024,7 +24023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="362" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A362" s="2" t="s">
         <v>526</v>
       </c>
@@ -24084,7 +24083,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="363" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A363" s="2" t="s">
         <v>527</v>
       </c>
@@ -24144,7 +24143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="364" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A364" s="2" t="s">
         <v>528</v>
       </c>
@@ -24204,7 +24203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="365" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A365" s="2" t="s">
         <v>529</v>
       </c>
@@ -24266,7 +24265,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="366" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A366" s="2" t="s">
         <v>532</v>
       </c>
@@ -24326,7 +24325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="367" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A367" s="2" t="s">
         <v>534</v>
       </c>
@@ -24386,7 +24385,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="368" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A368" s="2" t="s">
         <v>535</v>
       </c>
@@ -24448,7 +24447,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="369" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A369" s="2" t="s">
         <v>537</v>
       </c>
@@ -24510,7 +24509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="370" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A370" s="2" t="s">
         <v>538</v>
       </c>
@@ -24570,7 +24569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="371" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A371" s="2" t="s">
         <v>540</v>
       </c>
@@ -24630,7 +24629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="372" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A372" s="2" t="s">
         <v>542</v>
       </c>
@@ -24690,7 +24689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="373" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A373" s="2" t="s">
         <v>543</v>
       </c>
@@ -24750,7 +24749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="374" spans="1:20" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A374" s="2" t="s">
         <v>545</v>
       </c>
@@ -24808,7 +24807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="375" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A375" s="2" t="s">
         <v>548</v>
       </c>
@@ -24870,7 +24869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="376" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A376" s="2" t="s">
         <v>551</v>
       </c>
@@ -24932,7 +24931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="377" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A377" s="2" t="s">
         <v>553</v>
       </c>
@@ -24992,7 +24991,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="378" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A378" s="2" t="s">
         <v>557</v>
       </c>
@@ -25052,7 +25051,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="379" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A379" s="2" t="s">
         <v>558</v>
       </c>
@@ -25112,7 +25111,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="380" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A380" s="2" t="s">
         <v>559</v>
       </c>
@@ -25174,7 +25173,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="381" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A381" s="2" t="s">
         <v>562</v>
       </c>
@@ -25236,7 +25235,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="382" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A382" s="2" t="s">
         <v>565</v>
       </c>
@@ -25296,7 +25295,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="383" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A383" s="2" t="s">
         <v>567</v>
       </c>
@@ -25356,7 +25355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="384" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A384" s="2" t="s">
         <v>568</v>
       </c>
@@ -25416,7 +25415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="385" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A385" s="2" t="s">
         <v>571</v>
       </c>
@@ -25476,7 +25475,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="386" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A386" s="2" t="s">
         <v>572</v>
       </c>
@@ -25536,7 +25535,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="387" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A387" s="2" t="s">
         <v>573</v>
       </c>
@@ -25596,7 +25595,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="388" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A388" s="2" t="s">
         <v>574</v>
       </c>
@@ -25656,7 +25655,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="389" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A389" s="2" t="s">
         <v>575</v>
       </c>
@@ -25716,7 +25715,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="390" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A390" s="2" t="s">
         <v>576</v>
       </c>
@@ -25824,7 +25823,7 @@
       <c r="S392" s="2"/>
       <c r="T392" s="2"/>
     </row>
-    <row r="393" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A393" s="2" t="s">
         <v>576</v>
       </c>
@@ -25932,7 +25931,7 @@
       <c r="S395" s="2"/>
       <c r="T395" s="2"/>
     </row>
-    <row r="396" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A396" s="2" t="s">
         <v>576</v>
       </c>
@@ -26040,7 +26039,7 @@
       <c r="S398" s="2"/>
       <c r="T398" s="2"/>
     </row>
-    <row r="399" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A399" s="2" t="s">
         <v>576</v>
       </c>
@@ -26148,7 +26147,7 @@
       <c r="S401" s="2"/>
       <c r="T401" s="2"/>
     </row>
-    <row r="402" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A402" s="2" t="s">
         <v>576</v>
       </c>
@@ -26256,7 +26255,7 @@
       <c r="S404" s="2"/>
       <c r="T404" s="2"/>
     </row>
-    <row r="405" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A405" s="2" t="s">
         <v>576</v>
       </c>
@@ -26364,7 +26363,7 @@
       <c r="S407" s="2"/>
       <c r="T407" s="2"/>
     </row>
-    <row r="408" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A408" s="2" t="s">
         <v>576</v>
       </c>
@@ -26472,7 +26471,7 @@
       <c r="S410" s="2"/>
       <c r="T410" s="2"/>
     </row>
-    <row r="411" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A411" s="2" t="s">
         <v>576</v>
       </c>
@@ -26580,7 +26579,7 @@
       <c r="S413" s="2"/>
       <c r="T413" s="2"/>
     </row>
-    <row r="414" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A414" s="2" t="s">
         <v>576</v>
       </c>
@@ -26688,7 +26687,7 @@
       <c r="S416" s="2"/>
       <c r="T416" s="2"/>
     </row>
-    <row r="417" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A417" s="2" t="s">
         <v>576</v>
       </c>
@@ -26796,7 +26795,7 @@
       <c r="S419" s="2"/>
       <c r="T419" s="2"/>
     </row>
-    <row r="420" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A420" s="2" t="s">
         <v>576</v>
       </c>
@@ -26904,7 +26903,7 @@
       <c r="S422" s="2"/>
       <c r="T422" s="2"/>
     </row>
-    <row r="423" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A423" s="2" t="s">
         <v>576</v>
       </c>
@@ -27012,7 +27011,7 @@
       <c r="S425" s="2"/>
       <c r="T425" s="2"/>
     </row>
-    <row r="426" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A426" s="2" t="s">
         <v>576</v>
       </c>
@@ -27120,7 +27119,7 @@
       <c r="S428" s="2"/>
       <c r="T428" s="2"/>
     </row>
-    <row r="429" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A429" s="2" t="s">
         <v>576</v>
       </c>
@@ -27228,7 +27227,7 @@
       <c r="S431" s="2"/>
       <c r="T431" s="2"/>
     </row>
-    <row r="432" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A432" s="2" t="s">
         <v>576</v>
       </c>
@@ -27336,7 +27335,7 @@
       <c r="S434" s="2"/>
       <c r="T434" s="2"/>
     </row>
-    <row r="435" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A435" s="2" t="s">
         <v>576</v>
       </c>
@@ -27444,7 +27443,7 @@
       <c r="S437" s="2"/>
       <c r="T437" s="2"/>
     </row>
-    <row r="438" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A438" s="2" t="s">
         <v>576</v>
       </c>
@@ -27552,7 +27551,7 @@
       <c r="S440" s="2"/>
       <c r="T440" s="2"/>
     </row>
-    <row r="441" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A441" s="2" t="s">
         <v>576</v>
       </c>
@@ -27660,7 +27659,7 @@
       <c r="S443" s="2"/>
       <c r="T443" s="2"/>
     </row>
-    <row r="444" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A444" s="2" t="s">
         <v>576</v>
       </c>
@@ -27768,7 +27767,7 @@
       <c r="S446" s="2"/>
       <c r="T446" s="2"/>
     </row>
-    <row r="447" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A447" s="2" t="s">
         <v>576</v>
       </c>
@@ -27876,7 +27875,7 @@
       <c r="S449" s="2"/>
       <c r="T449" s="2"/>
     </row>
-    <row r="450" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A450" s="2" t="s">
         <v>576</v>
       </c>
@@ -27984,7 +27983,7 @@
       <c r="S452" s="2"/>
       <c r="T452" s="2"/>
     </row>
-    <row r="453" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A453" s="2" t="s">
         <v>576</v>
       </c>
@@ -28092,7 +28091,7 @@
       <c r="S455" s="2"/>
       <c r="T455" s="2"/>
     </row>
-    <row r="456" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A456" s="2" t="s">
         <v>576</v>
       </c>
@@ -28200,7 +28199,7 @@
       <c r="S458" s="2"/>
       <c r="T458" s="2"/>
     </row>
-    <row r="459" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A459" s="2" t="s">
         <v>576</v>
       </c>
@@ -28308,7 +28307,7 @@
       <c r="S461" s="2"/>
       <c r="T461" s="2"/>
     </row>
-    <row r="462" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A462" s="2" t="s">
         <v>576</v>
       </c>
@@ -28416,7 +28415,7 @@
       <c r="S464" s="2"/>
       <c r="T464" s="2"/>
     </row>
-    <row r="465" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A465" s="2" t="s">
         <v>576</v>
       </c>
@@ -28524,7 +28523,7 @@
       <c r="S467" s="2"/>
       <c r="T467" s="2"/>
     </row>
-    <row r="468" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A468" s="2" t="s">
         <v>576</v>
       </c>
@@ -28632,7 +28631,7 @@
       <c r="S470" s="2"/>
       <c r="T470" s="2"/>
     </row>
-    <row r="471" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A471" s="2" t="s">
         <v>576</v>
       </c>
@@ -28740,7 +28739,7 @@
       <c r="S473" s="2"/>
       <c r="T473" s="2"/>
     </row>
-    <row r="474" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A474" s="2" t="s">
         <v>576</v>
       </c>
@@ -28848,7 +28847,7 @@
       <c r="S476" s="2"/>
       <c r="T476" s="2"/>
     </row>
-    <row r="477" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A477" s="2" t="s">
         <v>576</v>
       </c>
@@ -28956,7 +28955,7 @@
       <c r="S479" s="2"/>
       <c r="T479" s="2"/>
     </row>
-    <row r="480" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A480" s="2" t="s">
         <v>576</v>
       </c>
@@ -29064,7 +29063,7 @@
       <c r="S482" s="2"/>
       <c r="T482" s="2"/>
     </row>
-    <row r="483" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A483" s="2" t="s">
         <v>576</v>
       </c>
@@ -29172,7 +29171,7 @@
       <c r="S485" s="2"/>
       <c r="T485" s="2"/>
     </row>
-    <row r="486" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A486" s="2" t="s">
         <v>576</v>
       </c>
@@ -29280,7 +29279,7 @@
       <c r="S488" s="2"/>
       <c r="T488" s="2"/>
     </row>
-    <row r="489" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A489" s="2" t="s">
         <v>576</v>
       </c>
@@ -29388,7 +29387,7 @@
       <c r="S491" s="2"/>
       <c r="T491" s="2"/>
     </row>
-    <row r="492" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A492" s="2" t="s">
         <v>576</v>
       </c>
@@ -29496,7 +29495,7 @@
       <c r="S494" s="2"/>
       <c r="T494" s="2"/>
     </row>
-    <row r="495" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A495" s="2" t="s">
         <v>576</v>
       </c>
@@ -29604,7 +29603,7 @@
       <c r="S497" s="2"/>
       <c r="T497" s="2"/>
     </row>
-    <row r="498" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A498" s="2" t="s">
         <v>576</v>
       </c>
@@ -29712,7 +29711,7 @@
       <c r="S500" s="2"/>
       <c r="T500" s="2"/>
     </row>
-    <row r="501" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A501" s="2" t="s">
         <v>576</v>
       </c>
@@ -29820,7 +29819,7 @@
       <c r="S503" s="2"/>
       <c r="T503" s="2"/>
     </row>
-    <row r="504" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="504" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A504" s="2" t="s">
         <v>576</v>
       </c>
@@ -29928,7 +29927,7 @@
       <c r="S506" s="2"/>
       <c r="T506" s="2"/>
     </row>
-    <row r="507" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="507" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A507" s="2" t="s">
         <v>576</v>
       </c>
@@ -30036,7 +30035,7 @@
       <c r="S509" s="2"/>
       <c r="T509" s="2"/>
     </row>
-    <row r="510" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="510" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A510" s="2" t="s">
         <v>576</v>
       </c>
@@ -30144,7 +30143,7 @@
       <c r="S512" s="2"/>
       <c r="T512" s="2"/>
     </row>
-    <row r="513" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="513" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A513" s="2" t="s">
         <v>576</v>
       </c>
@@ -30252,7 +30251,7 @@
       <c r="S515" s="2"/>
       <c r="T515" s="2"/>
     </row>
-    <row r="516" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="516" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A516" s="2" t="s">
         <v>576</v>
       </c>
@@ -30360,7 +30359,7 @@
       <c r="S518" s="2"/>
       <c r="T518" s="2"/>
     </row>
-    <row r="519" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="519" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A519" s="2" t="s">
         <v>576</v>
       </c>
@@ -30468,7 +30467,7 @@
       <c r="S521" s="2"/>
       <c r="T521" s="2"/>
     </row>
-    <row r="522" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="522" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A522" s="2" t="s">
         <v>576</v>
       </c>
@@ -30576,7 +30575,7 @@
       <c r="S524" s="2"/>
       <c r="T524" s="2"/>
     </row>
-    <row r="525" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="525" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A525" s="2" t="s">
         <v>576</v>
       </c>
@@ -30684,7 +30683,7 @@
       <c r="S527" s="2"/>
       <c r="T527" s="2"/>
     </row>
-    <row r="528" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="528" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A528" s="2" t="s">
         <v>576</v>
       </c>
@@ -30792,7 +30791,7 @@
       <c r="S530" s="2"/>
       <c r="T530" s="2"/>
     </row>
-    <row r="531" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="531" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A531" s="2" t="s">
         <v>576</v>
       </c>
@@ -30900,7 +30899,7 @@
       <c r="S533" s="2"/>
       <c r="T533" s="2"/>
     </row>
-    <row r="534" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="534" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A534" s="2" t="s">
         <v>576</v>
       </c>
@@ -31008,7 +31007,7 @@
       <c r="S536" s="2"/>
       <c r="T536" s="2"/>
     </row>
-    <row r="537" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="537" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A537" s="2" t="s">
         <v>576</v>
       </c>
@@ -31116,7 +31115,7 @@
       <c r="S539" s="2"/>
       <c r="T539" s="2"/>
     </row>
-    <row r="540" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="540" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A540" s="2" t="s">
         <v>576</v>
       </c>
@@ -31224,7 +31223,7 @@
       <c r="S542" s="2"/>
       <c r="T542" s="2"/>
     </row>
-    <row r="543" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="543" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A543" s="2" t="s">
         <v>576</v>
       </c>
@@ -31332,7 +31331,7 @@
       <c r="S545" s="2"/>
       <c r="T545" s="2"/>
     </row>
-    <row r="546" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="546" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A546" s="2" t="s">
         <v>577</v>
       </c>
@@ -31450,7 +31449,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="548" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="548" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A548" s="2" t="s">
         <v>579</v>
       </c>
@@ -31510,7 +31509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="549" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="549" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A549" s="2" t="s">
         <v>579</v>
       </c>
@@ -31570,7 +31569,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="550" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="550" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A550" s="2" t="s">
         <v>579</v>
       </c>
@@ -31632,7 +31631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="551" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="551" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A551" s="2" t="s">
         <v>580</v>
       </c>
@@ -31694,7 +31693,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="552" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="552" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A552" s="2" t="s">
         <v>580</v>
       </c>
@@ -31754,7 +31753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="553" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="553" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A553" s="2" t="s">
         <v>581</v>
       </c>
@@ -31816,7 +31815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="554" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="554" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A554" s="2" t="s">
         <v>582</v>
       </c>
@@ -31878,7 +31877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="555" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="555" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A555" s="2" t="s">
         <v>583</v>
       </c>
@@ -31940,7 +31939,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="556" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="556" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A556" s="2" t="s">
         <v>584</v>
       </c>
@@ -32002,7 +32001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="557" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="557" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A557" s="2" t="s">
         <v>585</v>
       </c>
@@ -32064,7 +32063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="558" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="558" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A558" s="2" t="s">
         <v>586</v>
       </c>
@@ -32126,7 +32125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="559" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="559" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A559" s="2" t="s">
         <v>587</v>
       </c>
@@ -32186,7 +32185,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="560" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="560" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A560" s="2" t="s">
         <v>588</v>
       </c>
@@ -32246,7 +32245,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="561" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="561" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A561" s="2" t="s">
         <v>589</v>
       </c>
@@ -32304,7 +32303,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="562" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="562" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A562" s="2" t="s">
         <v>590</v>
       </c>
@@ -32362,7 +32361,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="563" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="563" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A563" s="2" t="s">
         <v>591</v>
       </c>
@@ -32420,7 +32419,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="564" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="564" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A564" s="2" t="s">
         <v>592</v>
       </c>
@@ -32480,7 +32479,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="565" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="565" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A565" s="2" t="s">
         <v>593</v>
       </c>
@@ -32586,7 +32585,7 @@
       <c r="S567" s="2"/>
       <c r="T567" s="2"/>
     </row>
-    <row r="568" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="568" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A568" s="2"/>
       <c r="B568" s="2" t="s">
         <v>525</v>
@@ -32640,7 +32639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="569" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="569" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A569" s="2"/>
       <c r="B569" s="2" t="s">
         <v>525</v>
@@ -32694,7 +32693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="570" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="570" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A570" s="2"/>
       <c r="B570" s="2" t="s">
         <v>525</v>
@@ -32748,7 +32747,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="571" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="571" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A571" s="2"/>
       <c r="B571" s="2" t="s">
         <v>525</v>
@@ -32802,7 +32801,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="572" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="572" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A572" s="2"/>
       <c r="B572" s="2" t="s">
         <v>525</v>
@@ -32856,7 +32855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="573" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="573" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A573" s="2"/>
       <c r="B573" s="2" t="s">
         <v>525</v>
@@ -32910,7 +32909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="574" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="574" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A574" s="2"/>
       <c r="B574" s="2" t="s">
         <v>525</v>
@@ -32964,7 +32963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="575" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="575" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A575" s="2"/>
       <c r="B575" s="2" t="s">
         <v>525</v>
@@ -33018,7 +33017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="576" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="576" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A576" s="2"/>
       <c r="B576" s="2" t="s">
         <v>525</v>
@@ -33072,7 +33071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="577" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="577" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A577" s="2"/>
       <c r="B577" s="2" t="s">
         <v>525</v>
@@ -33126,7 +33125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="578" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="578" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A578" s="2"/>
       <c r="B578" s="2" t="s">
         <v>525</v>
@@ -33180,7 +33179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="579" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="579" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A579" s="2"/>
       <c r="B579" s="2" t="s">
         <v>525</v>
@@ -33234,7 +33233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="580" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="580" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A580" s="2"/>
       <c r="B580" s="2" t="s">
         <v>525</v>
@@ -33288,7 +33287,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="581" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="581" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A581" s="2"/>
       <c r="B581" s="2" t="s">
         <v>525</v>
@@ -33342,7 +33341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="582" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="582" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A582" s="2"/>
       <c r="B582" s="2" t="s">
         <v>525</v>
@@ -33396,7 +33395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="583" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="583" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A583" s="2"/>
       <c r="B583" s="2" t="s">
         <v>525</v>
@@ -33450,7 +33449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="584" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="584" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A584" s="2"/>
       <c r="B584" s="2" t="s">
         <v>525</v>
@@ -33504,7 +33503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="585" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="585" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A585" s="2"/>
       <c r="B585" s="2" t="s">
         <v>525</v>
@@ -33558,7 +33557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="586" spans="1:20" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="586" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A586" s="2"/>
       <c r="B586" s="2" t="s">
         <v>525</v>
@@ -33613,11 +33612,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D586" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <filterColumn colId="0">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="D1:D586" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>